<commit_message>
added code to process seepage data in slice generation. this completes seepage implementation. moved some mesh plotting to plot.py.
</commit_message>
<xml_diff>
--- a/inputs/slope/input_template_lface4.xlsx
+++ b/inputs/slope/input_template_lface4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/CursorProjects/xslope/inputs/slope/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0226DB0-CF53-6A45-9943-ECBD50267D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F4E577-4C0D-0241-BBA7-D1350E029651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="20140" activeTab="3" xr2:uid="{BA54C293-CE08-6E4C-9212-B3317DAA148E}"/>
   </bookViews>
@@ -5808,16 +5808,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="M22:N22"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5828,7 +5828,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="K5" sqref="K5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5969,7 +5969,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -6017,7 +6017,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -6065,7 +6065,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>

</xml_diff>